<commit_message>
feat(users): ability to sync users with their groups (teacher or student)
</commit_message>
<xml_diff>
--- a/tests/data/users-import.xlsx
+++ b/tests/data/users-import.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\pm2etml-intranet\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\codespace\web\pm2etml-intranet\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="0" windowWidth="24120" windowHeight="11490"/>
+    <workbookView xWindow="10950" yWindow="0" windowWidth="24120" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="profs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>email</t>
   </si>
@@ -63,7 +63,103 @@
     <t>py6@eduvaud.ch</t>
   </si>
   <si>
-    <t>root,eleve,mp,doyen</t>
+    <t>period</t>
+  </si>
+  <si>
+    <t>fin1</t>
+  </si>
+  <si>
+    <t>root,mp,doyen</t>
+  </si>
+  <si>
+    <t>studfn</t>
+  </si>
+  <si>
+    <t>studln</t>
+  </si>
+  <si>
+    <t>studfnln@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>px89@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>eleve</t>
+  </si>
+  <si>
+    <t>cin1a</t>
+  </si>
+  <si>
+    <t>stud2fn</t>
+  </si>
+  <si>
+    <t>stud2ln</t>
+  </si>
+  <si>
+    <t>stud2@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>px2@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>cin2a</t>
+  </si>
+  <si>
+    <t>redoublé</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>already existing</t>
+  </si>
+  <si>
+    <t>samefn</t>
+  </si>
+  <si>
+    <t>sameln</t>
+  </si>
+  <si>
+    <t>samemail@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>same@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>cin2b</t>
+  </si>
+  <si>
+    <t>login@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>prof</t>
+  </si>
+  <si>
+    <t>modiffn</t>
+  </si>
+  <si>
+    <t>modifln</t>
+  </si>
+  <si>
+    <t>modif@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>fin2</t>
+  </si>
+  <si>
+    <t>erreur</t>
+  </si>
+  <si>
+    <t>erreur@erreur.com</t>
+  </si>
+  <si>
+    <t>FIN1</t>
+  </si>
+  <si>
+    <t>CIN2B</t>
   </si>
 </sst>
 </file>
@@ -556,9 +652,10 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -881,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +991,7 @@
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -910,8 +1007,17 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -927,31 +1033,279 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="2">
+        <v>44774</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="2">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="2">
+        <v>44409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="2">
+        <v>44774</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="2">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="2">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="2">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="2">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="2">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="D6" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="C12" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10"/>
+    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="C16" r:id="rId13"/>
+    <hyperlink ref="D16" r:id="rId14"/>
+    <hyperlink ref="C19" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(user sync): handle deleted/restored users
</commit_message>
<xml_diff>
--- a/tests/data/users-import.xlsx
+++ b/tests/data/users-import.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10950" yWindow="0" windowWidth="24120" windowHeight="11490"/>
+    <workbookView xWindow="16500" yWindow="0" windowWidth="9810" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="profs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t>email</t>
   </si>
@@ -160,6 +160,39 @@
   </si>
   <si>
     <t>CIN2B</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>tbd@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>cin1c</t>
+  </si>
+  <si>
+    <t>ruppture</t>
+  </si>
+  <si>
+    <t>ghost</t>
+  </si>
+  <si>
+    <t>ghost@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>rupture</t>
+  </si>
+  <si>
+    <t>bla ruPture au 748</t>
+  </si>
+  <si>
+    <t>tbr</t>
+  </si>
+  <si>
+    <t>tbr@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>min1</t>
   </si>
 </sst>
 </file>
@@ -978,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1286,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>37</v>
@@ -1268,12 +1301,12 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1285,6 +1318,127 @@
       </c>
       <c r="E19" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="2">
+        <v>44774</v>
+      </c>
+      <c r="H21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="2">
+        <v>44774</v>
+      </c>
+      <c r="H22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="2">
+        <v>44774</v>
+      </c>
+      <c r="H24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="2">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="2">
+        <v>44774</v>
+      </c>
+      <c r="H28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="2">
+        <v>44774</v>
       </c>
     </row>
   </sheetData>
@@ -1304,8 +1458,18 @@
     <hyperlink ref="C16" r:id="rId13"/>
     <hyperlink ref="D16" r:id="rId14"/>
     <hyperlink ref="C19" r:id="rId15"/>
+    <hyperlink ref="C21" r:id="rId16"/>
+    <hyperlink ref="D21" r:id="rId17"/>
+    <hyperlink ref="D22" r:id="rId18"/>
+    <hyperlink ref="C24" r:id="rId19"/>
+    <hyperlink ref="D24" r:id="rId20"/>
+    <hyperlink ref="C27" r:id="rId21"/>
+    <hyperlink ref="D27" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="C29" r:id="rId24"/>
+    <hyperlink ref="D29" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(mutation): keep evaluation history upon student migration (min->cin for instance...)
</commit_message>
<xml_diff>
--- a/tests/data/users-import.xlsx
+++ b/tests/data/users-import.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\codespace\web\pm2etml-intranet\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws\code\web\pm2etml-intranet\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="0" windowWidth="9810" windowHeight="11490"/>
+    <workbookView xWindow="17430" yWindow="0" windowWidth="9810" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="profs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>email</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>min1</t>
+  </si>
+  <si>
+    <t>migration depuis min2</t>
+  </si>
+  <si>
+    <t>migrator@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>tor</t>
+  </si>
+  <si>
+    <t>migra</t>
   </si>
 </sst>
 </file>
@@ -1011,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="A31" sqref="A31:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,6 +1451,30 @@
       </c>
       <c r="G29" s="2">
         <v>44774</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1468,8 +1504,10 @@
     <hyperlink ref="D28" r:id="rId23"/>
     <hyperlink ref="C29" r:id="rId24"/>
     <hyperlink ref="D29" r:id="rId25"/>
+    <hyperlink ref="C31" r:id="rId26"/>
+    <hyperlink ref="D31" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(test): migrator test user forced to 2022 period
</commit_message>
<xml_diff>
--- a/tests/data/users-import.xlsx
+++ b/tests/data/users-import.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17430" yWindow="0" windowWidth="9810" windowHeight="11490"/>
+    <workbookView xWindow="18360" yWindow="0" windowWidth="9810" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="profs" sheetId="1" r:id="rId1"/>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:I31"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,7 +1472,9 @@
       <c r="F31" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2">
+        <v>44774</v>
+      </c>
       <c r="H31" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
feat(repetition): auto removes contracts for students that repeat (redoublement)
</commit_message>
<xml_diff>
--- a/tests/data/users-import.xlsx
+++ b/tests/data/users-import.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws\code\web\pm2etml-intranet\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28542F2-B2F0-4492-BCDF-338AEC3D86C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18360" yWindow="0" windowWidth="9810" windowHeight="11490"/>
+    <workbookView xWindow="1140" yWindow="-120" windowWidth="27780" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="profs" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>email</t>
   </si>
@@ -205,12 +206,21 @@
   </si>
   <si>
     <t>migra</t>
+  </si>
+  <si>
+    <t>rep@eduvaud.ch</t>
+  </si>
+  <si>
+    <t>cin1b</t>
+  </si>
+  <si>
+    <t>missing redob</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1022,11 +1032,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="A33" sqref="A33:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,37 +1489,60 @@
         <v>58</v>
       </c>
     </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="2">
+        <v>44774</v>
+      </c>
+      <c r="H34" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="D4" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="D6" r:id="rId6"/>
-    <hyperlink ref="C9" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="C12" r:id="rId9"/>
-    <hyperlink ref="D12" r:id="rId10"/>
-    <hyperlink ref="D14" r:id="rId11"/>
-    <hyperlink ref="D15" r:id="rId12"/>
-    <hyperlink ref="C16" r:id="rId13"/>
-    <hyperlink ref="D16" r:id="rId14"/>
-    <hyperlink ref="C19" r:id="rId15"/>
-    <hyperlink ref="C21" r:id="rId16"/>
-    <hyperlink ref="D21" r:id="rId17"/>
-    <hyperlink ref="D22" r:id="rId18"/>
-    <hyperlink ref="C24" r:id="rId19"/>
-    <hyperlink ref="D24" r:id="rId20"/>
-    <hyperlink ref="C27" r:id="rId21"/>
-    <hyperlink ref="D27" r:id="rId22"/>
-    <hyperlink ref="D28" r:id="rId23"/>
-    <hyperlink ref="C29" r:id="rId24"/>
-    <hyperlink ref="D29" r:id="rId25"/>
-    <hyperlink ref="C31" r:id="rId26"/>
-    <hyperlink ref="D31" r:id="rId27"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C27" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D27" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C29" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D34" r:id="rId28" xr:uid="{512F7035-D689-4A7A-A35B-AFB32531076A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>